<commit_message>
fixing filenames, added missing runnumber to 4500 spikein
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_09.21.20.xlsx
+++ b/fastqFiles/fastq_09.21.20.xlsx
@@ -172,7 +172,7 @@
     <t xml:space="preserve">Brent_Exp27_6_GTAC_44_SIC_Index2_06_AACGGAGATC_GACCTTGT_S32_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">Brent_Exp27_7_GTAC_45_SIC_Index2_06_GATAGTTATC_GACCTTGT_S33_R1_001.fastq.gz:</t>
+    <t xml:space="preserve">Brent_Exp27_7_GTAC_45_SIC_Index2_06_GATAGTTATC_GACCTTGT_S33_R1_001.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">Brent_Exp27_8_GTAC_46_SIC_Index2_06_GGTGAATATC_GACCTTGT_S34_R1_001.fastq.gz</t>
@@ -406,15 +406,15 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N35" activeCellId="0" sqref="N35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.61"/>
   </cols>

</xml_diff>

<commit_message>
adding manual pass to sample
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_09.21.20.xlsx
+++ b/fastqFiles/fastq_09.21.20.xlsx
@@ -326,13 +326,17 @@
   </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X14" activeCellId="0" sqref="X14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="85.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,6 +1501,9 @@
       </c>
       <c r="L33" s="0" t="s">
         <v>53</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
adding manual review notes from 20200104
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_09.21.20.xlsx
+++ b/fastqFiles/fastq_09.21.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="70">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Brent_Exp25_8_GTAC_15_SIC_Index2_08_GGTCCTCATC_AAGCACGT_S9_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[512]</t>
   </si>
   <si>
     <t xml:space="preserve">Brent_Exp25_12_GTAC_20_SIC_Index2_08_ACAGATAATC_AAGCACGT_S10_R1_001.fastq.gz</t>
@@ -326,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L45" activeCellId="0" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,7 +338,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="85.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -662,6 +665,12 @@
       <c r="L9" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -695,10 +704,10 @@
         <v>7275284</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>14</v>
       </c>
@@ -730,7 +739,13 @@
         <v>10479552</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +780,7 @@
         <v>7422146</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,7 +815,7 @@
         <v>8540709</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,7 +850,7 @@
         <v>8042588</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +885,7 @@
         <v>5506110</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +920,13 @@
         <v>8430712</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,7 +961,7 @@
         <v>8572772</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,15 +996,15 @@
         <v>7837403</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -1010,15 +1031,15 @@
         <v>7432288</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2</v>
@@ -1045,15 +1066,15 @@
         <v>7004200</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>3</v>
@@ -1080,15 +1101,15 @@
         <v>13956454</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>4</v>
@@ -1115,15 +1136,15 @@
         <v>7357291</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>5</v>
@@ -1150,15 +1171,15 @@
         <v>8315277</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>6</v>
@@ -1185,15 +1206,15 @@
         <v>7600411</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>7</v>
@@ -1220,15 +1241,15 @@
         <v>9388582</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>8</v>
@@ -1255,12 +1276,12 @@
         <v>8225970</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>15</v>
@@ -1290,12 +1311,12 @@
         <v>9532904</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>15</v>
@@ -1325,12 +1346,12 @@
         <v>9489424</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>15</v>
@@ -1360,12 +1381,12 @@
         <v>11199294</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>15</v>
@@ -1395,12 +1416,12 @@
         <v>8732031</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>15</v>
@@ -1430,12 +1451,12 @@
         <v>7804640</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>15</v>
@@ -1465,12 +1486,12 @@
         <v>11042637</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>15</v>
@@ -1500,15 +1521,15 @@
         <v>8955279</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>15</v>
@@ -1538,12 +1559,18 @@
         <v>9652956</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>15</v>
@@ -1573,12 +1600,12 @@
         <v>1778922</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>15</v>
@@ -1608,12 +1635,12 @@
         <v>8707856</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>15</v>
@@ -1643,12 +1670,12 @@
         <v>8771886</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>15</v>
@@ -1678,12 +1705,12 @@
         <v>8670204</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>15</v>
@@ -1713,12 +1740,12 @@
         <v>8901341</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>15</v>
@@ -1748,12 +1775,12 @@
         <v>7649468</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>15</v>
@@ -1783,12 +1810,12 @@
         <v>8486185</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>15</v>
@@ -1818,12 +1845,12 @@
         <v>8254384</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>15</v>
@@ -1853,12 +1880,12 @@
         <v>9455887</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>15</v>
@@ -1888,12 +1915,12 @@
         <v>9712269</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>15</v>
@@ -1923,12 +1950,18 @@
         <v>7648415</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N45" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>15</v>
@@ -1958,12 +1991,12 @@
         <v>9480975</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>15</v>
@@ -1993,12 +2026,12 @@
         <v>7974154</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>15</v>
@@ -2028,7 +2061,7 @@
         <v>9507221</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>